<commit_message>
Fixed a typo in the 384-well example file.
</commit_message>
<xml_diff>
--- a/inst/extdata/input_files/test384.xlsx
+++ b/inst/extdata/input_files/test384.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gage1\Documents\Work\RTQ_analysis\tests\testthat\input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowde002\Documents\quicR\inst\extdata\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A400B51A-870D-417B-982C-8F5EDE8C7340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A228A9-BB06-4443-B0DF-0B7653FD8988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate Cycle 1 (0 h)" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="430">
   <si>
     <t>User: USER</t>
   </si>
@@ -1544,7 +1544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1600,9 +1600,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6260,8 +6257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:JF80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10302,7 +10299,9 @@
       </c>
     </row>
     <row r="16" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
@@ -11100,7 +11099,9 @@
       </c>
     </row>
     <row r="17" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B17" s="1">
         <v>0.75</v>
       </c>
@@ -11898,7 +11899,9 @@
       </c>
     </row>
     <row r="18" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B18" s="1">
         <v>1.5</v>
       </c>
@@ -12696,7 +12699,9 @@
       </c>
     </row>
     <row r="19" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B19" s="1">
         <v>2.25</v>
       </c>
@@ -13494,7 +13499,9 @@
       </c>
     </row>
     <row r="20" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -14292,7 +14299,9 @@
       </c>
     </row>
     <row r="21" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B21" s="1">
         <v>3.75</v>
       </c>
@@ -15090,7 +15099,9 @@
       </c>
     </row>
     <row r="22" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B22" s="1">
         <v>4.5</v>
       </c>
@@ -15888,7 +15899,9 @@
       </c>
     </row>
     <row r="23" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B23" s="1">
         <v>5.25</v>
       </c>
@@ -16686,7 +16699,9 @@
       </c>
     </row>
     <row r="24" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B24" s="1">
         <v>6</v>
       </c>
@@ -17484,7 +17499,9 @@
       </c>
     </row>
     <row r="25" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B25" s="1">
         <v>6.75</v>
       </c>
@@ -18282,7 +18299,9 @@
       </c>
     </row>
     <row r="26" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B26" s="1">
         <v>7.5</v>
       </c>
@@ -19080,7 +19099,9 @@
       </c>
     </row>
     <row r="27" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B27" s="1">
         <v>8.25</v>
       </c>
@@ -19878,7 +19899,9 @@
       </c>
     </row>
     <row r="28" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B28" s="1">
         <v>9</v>
       </c>
@@ -20676,7 +20699,9 @@
       </c>
     </row>
     <row r="29" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B29" s="1">
         <v>9.75</v>
       </c>
@@ -21474,7 +21499,9 @@
       </c>
     </row>
     <row r="30" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B30" s="1">
         <v>10.5</v>
       </c>
@@ -22272,7 +22299,9 @@
       </c>
     </row>
     <row r="31" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B31" s="1">
         <v>11.25</v>
       </c>
@@ -23070,7 +23099,9 @@
       </c>
     </row>
     <row r="32" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B32" s="1">
         <v>12</v>
       </c>
@@ -23868,7 +23899,9 @@
       </c>
     </row>
     <row r="33" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B33" s="1">
         <v>12.75</v>
       </c>
@@ -24666,7 +24699,9 @@
       </c>
     </row>
     <row r="34" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B34" s="1">
         <v>13.5</v>
       </c>
@@ -25464,7 +25499,9 @@
       </c>
     </row>
     <row r="35" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B35" s="1">
         <v>14.25</v>
       </c>
@@ -26262,7 +26299,9 @@
       </c>
     </row>
     <row r="36" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B36" s="1">
         <v>15</v>
       </c>
@@ -27060,7 +27099,9 @@
       </c>
     </row>
     <row r="37" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B37" s="1">
         <v>15.75</v>
       </c>
@@ -27858,7 +27899,9 @@
       </c>
     </row>
     <row r="38" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B38" s="1">
         <v>16.5</v>
       </c>
@@ -28656,7 +28699,9 @@
       </c>
     </row>
     <row r="39" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B39" s="1">
         <v>17.25</v>
       </c>
@@ -29454,7 +29499,9 @@
       </c>
     </row>
     <row r="40" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B40" s="1">
         <v>18</v>
       </c>
@@ -30252,7 +30299,9 @@
       </c>
     </row>
     <row r="41" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B41" s="1">
         <v>18.75</v>
       </c>
@@ -31050,7 +31099,9 @@
       </c>
     </row>
     <row r="42" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B42" s="1">
         <v>19.5</v>
       </c>
@@ -31848,7 +31899,9 @@
       </c>
     </row>
     <row r="43" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B43" s="1">
         <v>20.25</v>
       </c>
@@ -32646,7 +32699,9 @@
       </c>
     </row>
     <row r="44" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B44" s="1">
         <v>21</v>
       </c>
@@ -33444,7 +33499,9 @@
       </c>
     </row>
     <row r="45" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B45" s="1">
         <v>21.75</v>
       </c>
@@ -34242,7 +34299,9 @@
       </c>
     </row>
     <row r="46" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B46" s="1">
         <v>22.5</v>
       </c>
@@ -35040,7 +35099,9 @@
       </c>
     </row>
     <row r="47" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+      <c r="A47" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B47" s="1">
         <v>23.25</v>
       </c>
@@ -35838,7 +35899,9 @@
       </c>
     </row>
     <row r="48" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B48" s="1">
         <v>24</v>
       </c>
@@ -36636,7 +36699,9 @@
       </c>
     </row>
     <row r="49" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B49" s="1">
         <v>24.75</v>
       </c>
@@ -37434,7 +37499,9 @@
       </c>
     </row>
     <row r="50" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B50" s="1">
         <v>25.5</v>
       </c>
@@ -38232,7 +38299,9 @@
       </c>
     </row>
     <row r="51" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+      <c r="A51" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B51" s="1">
         <v>26.25</v>
       </c>
@@ -39030,7 +39099,9 @@
       </c>
     </row>
     <row r="52" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B52" s="1">
         <v>27</v>
       </c>
@@ -39828,7 +39899,9 @@
       </c>
     </row>
     <row r="53" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B53" s="1">
         <v>27.75</v>
       </c>
@@ -40626,7 +40699,9 @@
       </c>
     </row>
     <row r="54" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
+      <c r="A54" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B54" s="1">
         <v>28.5</v>
       </c>
@@ -41424,7 +41499,9 @@
       </c>
     </row>
     <row r="55" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+      <c r="A55" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B55" s="1">
         <v>29.25</v>
       </c>
@@ -42222,7 +42299,9 @@
       </c>
     </row>
     <row r="56" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
+      <c r="A56" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B56" s="1">
         <v>30</v>
       </c>
@@ -43020,7 +43099,9 @@
       </c>
     </row>
     <row r="57" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B57" s="1">
         <v>30.75</v>
       </c>
@@ -43818,7 +43899,9 @@
       </c>
     </row>
     <row r="58" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
+      <c r="A58" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B58" s="1">
         <v>31.5</v>
       </c>
@@ -44616,7 +44699,9 @@
       </c>
     </row>
     <row r="59" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B59" s="1">
         <v>32.25</v>
       </c>
@@ -45414,7 +45499,9 @@
       </c>
     </row>
     <row r="60" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+      <c r="A60" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B60" s="1">
         <v>33</v>
       </c>
@@ -46212,7 +46299,9 @@
       </c>
     </row>
     <row r="61" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B61" s="1">
         <v>33.75</v>
       </c>
@@ -47010,7 +47099,9 @@
       </c>
     </row>
     <row r="62" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B62" s="1">
         <v>34.5</v>
       </c>
@@ -47808,7 +47899,9 @@
       </c>
     </row>
     <row r="63" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+      <c r="A63" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B63" s="1">
         <v>35.25</v>
       </c>
@@ -48606,7 +48699,9 @@
       </c>
     </row>
     <row r="64" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
+      <c r="A64" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B64" s="1">
         <v>36</v>
       </c>
@@ -49404,7 +49499,9 @@
       </c>
     </row>
     <row r="65" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
+      <c r="A65" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B65" s="1">
         <v>36.75</v>
       </c>
@@ -50202,7 +50299,9 @@
       </c>
     </row>
     <row r="66" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+      <c r="A66" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B66" s="1">
         <v>37.5</v>
       </c>
@@ -51000,7 +51099,9 @@
       </c>
     </row>
     <row r="67" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
+      <c r="A67" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B67" s="1">
         <v>38.25</v>
       </c>
@@ -51798,7 +51899,9 @@
       </c>
     </row>
     <row r="68" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
+      <c r="A68" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B68" s="1">
         <v>39</v>
       </c>
@@ -52596,7 +52699,9 @@
       </c>
     </row>
     <row r="69" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
+      <c r="A69" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B69" s="1">
         <v>39.75</v>
       </c>
@@ -53394,7 +53499,9 @@
       </c>
     </row>
     <row r="70" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B70" s="1">
         <v>40.5</v>
       </c>
@@ -54192,7 +54299,9 @@
       </c>
     </row>
     <row r="71" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B71" s="1">
         <v>41.25</v>
       </c>
@@ -54990,7 +55099,9 @@
       </c>
     </row>
     <row r="72" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B72" s="1">
         <v>42</v>
       </c>
@@ -55788,7 +55899,9 @@
       </c>
     </row>
     <row r="73" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
+      <c r="A73" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B73" s="1">
         <v>42.75</v>
       </c>
@@ -56586,7 +56699,9 @@
       </c>
     </row>
     <row r="74" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B74" s="1">
         <v>43.5</v>
       </c>
@@ -57384,7 +57499,9 @@
       </c>
     </row>
     <row r="75" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
+      <c r="A75" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B75" s="1">
         <v>44.25</v>
       </c>
@@ -58182,7 +58299,9 @@
       </c>
     </row>
     <row r="76" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
+      <c r="A76" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B76" s="1">
         <v>45</v>
       </c>
@@ -58980,7 +59099,9 @@
       </c>
     </row>
     <row r="77" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B77" s="1">
         <v>45.75</v>
       </c>
@@ -59778,7 +59899,9 @@
       </c>
     </row>
     <row r="78" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
+      <c r="A78" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B78" s="1">
         <v>46.5</v>
       </c>
@@ -60576,7 +60699,9 @@
       </c>
     </row>
     <row r="79" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
+      <c r="A79" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B79" s="1">
         <v>47.25</v>
       </c>
@@ -61374,7 +61499,9 @@
       </c>
     </row>
     <row r="80" spans="1:266" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
+      <c r="A80" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="B80" s="1">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Added raw files for benchmarking against QuICSeedR.
</commit_message>
<xml_diff>
--- a/inst/extdata/input_files/test384.xlsx
+++ b/inst/extdata/input_files/test384.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowde002\Documents\quicR\inst\extdata\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A228A9-BB06-4443-B0DF-0B7653FD8988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119D4213-3C81-4D17-9873-A43E8410481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate Cycle 1 (0 h)" sheetId="2" r:id="rId1"/>
@@ -1544,7 +1544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1601,6 +1601,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1884,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AA88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5263,990 +5266,990 @@
       <c r="B73" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F73" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="G73" s="8" t="s">
+      <c r="G73" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="H73" s="8" t="s">
+      <c r="H73" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="I73" s="8" t="s">
+      <c r="I73" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="J73" s="8" t="s">
+      <c r="J73" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="K73" s="8" t="s">
+      <c r="K73" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="L73" s="8" t="s">
+      <c r="L73" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="M73" s="8" t="s">
+      <c r="M73" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="N73" s="8" t="s">
+      <c r="N73" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="O73" s="8" t="s">
+      <c r="O73" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="P73" s="8" t="s">
+      <c r="P73" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="8"/>
-      <c r="S73" s="8"/>
-      <c r="T73" s="8"/>
-      <c r="U73" s="8"/>
-      <c r="V73" s="8"/>
-      <c r="W73" s="8"/>
-      <c r="X73" s="8"/>
-      <c r="Y73" s="8"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="9"/>
+      <c r="S73" s="9"/>
+      <c r="T73" s="9"/>
+      <c r="U73" s="9"/>
+      <c r="V73" s="9"/>
+      <c r="W73" s="9"/>
+      <c r="X73" s="9"/>
+      <c r="Y73" s="10"/>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="G74" s="8" t="s">
+      <c r="G74" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="H74" s="8" t="s">
+      <c r="H74" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="I74" s="8" t="s">
+      <c r="I74" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="J74" s="8" t="s">
+      <c r="J74" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="K74" s="8" t="s">
+      <c r="K74" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="L74" s="8" t="s">
+      <c r="L74" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="M74" s="8" t="s">
+      <c r="M74" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="N74" s="8" t="s">
+      <c r="N74" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="O74" s="8" t="s">
+      <c r="O74" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="P74" s="8" t="s">
+      <c r="P74" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="Q74" s="8"/>
-      <c r="R74" s="8"/>
-      <c r="S74" s="8"/>
-      <c r="T74" s="8"/>
-      <c r="U74" s="8"/>
-      <c r="V74" s="8"/>
-      <c r="W74" s="8"/>
-      <c r="X74" s="8"/>
-      <c r="Y74" s="8"/>
+      <c r="Q74" s="23"/>
+      <c r="R74" s="23"/>
+      <c r="S74" s="23"/>
+      <c r="T74" s="23"/>
+      <c r="U74" s="23"/>
+      <c r="V74" s="23"/>
+      <c r="W74" s="23"/>
+      <c r="X74" s="23"/>
+      <c r="Y74" s="12"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F75" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="G75" s="8" t="s">
+      <c r="G75" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="H75" s="8" t="s">
+      <c r="H75" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="I75" s="8" t="s">
+      <c r="I75" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="J75" s="8" t="s">
+      <c r="J75" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="K75" s="8" t="s">
+      <c r="K75" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="L75" s="8" t="s">
+      <c r="L75" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="M75" s="8" t="s">
+      <c r="M75" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="N75" s="8" t="s">
+      <c r="N75" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="O75" s="8" t="s">
+      <c r="O75" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="P75" s="8" t="s">
+      <c r="P75" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="Q75" s="8"/>
-      <c r="R75" s="8"/>
-      <c r="S75" s="8"/>
-      <c r="T75" s="8"/>
-      <c r="U75" s="8"/>
-      <c r="V75" s="8"/>
-      <c r="W75" s="8"/>
-      <c r="X75" s="8"/>
-      <c r="Y75" s="8"/>
+      <c r="Q75" s="23"/>
+      <c r="R75" s="23"/>
+      <c r="S75" s="23"/>
+      <c r="T75" s="23"/>
+      <c r="U75" s="23"/>
+      <c r="V75" s="23"/>
+      <c r="W75" s="23"/>
+      <c r="X75" s="23"/>
+      <c r="Y75" s="12"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="F76" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="G76" s="8" t="s">
+      <c r="G76" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="H76" s="8" t="s">
+      <c r="H76" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="I76" s="8" t="s">
+      <c r="I76" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="J76" s="8" t="s">
+      <c r="J76" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="K76" s="8" t="s">
+      <c r="K76" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="L76" s="8" t="s">
+      <c r="L76" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="M76" s="8" t="s">
+      <c r="M76" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="N76" s="8" t="s">
+      <c r="N76" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="O76" s="8" t="s">
+      <c r="O76" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="P76" s="8" t="s">
+      <c r="P76" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="Q76" s="8"/>
-      <c r="R76" s="8"/>
-      <c r="S76" s="8"/>
-      <c r="T76" s="8"/>
-      <c r="U76" s="8"/>
-      <c r="V76" s="8"/>
-      <c r="W76" s="8"/>
-      <c r="X76" s="8"/>
-      <c r="Y76" s="8"/>
+      <c r="Q76" s="23"/>
+      <c r="R76" s="23"/>
+      <c r="S76" s="23"/>
+      <c r="T76" s="23"/>
+      <c r="U76" s="23"/>
+      <c r="V76" s="23"/>
+      <c r="W76" s="23"/>
+      <c r="X76" s="23"/>
+      <c r="Y76" s="12"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="E77" s="8" t="s">
+      <c r="E77" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="F77" s="8" t="s">
+      <c r="F77" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="G77" s="8" t="s">
+      <c r="G77" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="H77" s="8" t="s">
+      <c r="H77" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="I77" s="8" t="s">
+      <c r="I77" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="J77" s="8" t="s">
+      <c r="J77" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="K77" s="8" t="s">
+      <c r="K77" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="L77" s="8" t="s">
+      <c r="L77" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="M77" s="8" t="s">
+      <c r="M77" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="N77" s="8" t="s">
+      <c r="N77" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="O77" s="8" t="s">
+      <c r="O77" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="P77" s="8" t="s">
+      <c r="P77" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="Q77" s="8"/>
-      <c r="R77" s="8"/>
-      <c r="S77" s="8"/>
-      <c r="T77" s="8"/>
-      <c r="U77" s="8"/>
-      <c r="V77" s="8"/>
-      <c r="W77" s="8"/>
-      <c r="X77" s="8"/>
-      <c r="Y77" s="8"/>
+      <c r="Q77" s="23"/>
+      <c r="R77" s="23"/>
+      <c r="S77" s="23"/>
+      <c r="T77" s="23"/>
+      <c r="U77" s="23"/>
+      <c r="V77" s="23"/>
+      <c r="W77" s="23"/>
+      <c r="X77" s="23"/>
+      <c r="Y77" s="12"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="E78" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="F78" s="8" t="s">
+      <c r="F78" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="G78" s="8" t="s">
+      <c r="G78" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="H78" s="8" t="s">
+      <c r="H78" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="I78" s="8" t="s">
+      <c r="I78" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="J78" s="8" t="s">
+      <c r="J78" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="K78" s="8" t="s">
+      <c r="K78" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="L78" s="8" t="s">
+      <c r="L78" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="M78" s="8" t="s">
+      <c r="M78" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="N78" s="8" t="s">
+      <c r="N78" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="O78" s="8" t="s">
+      <c r="O78" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="P78" s="8" t="s">
+      <c r="P78" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="Q78" s="8"/>
-      <c r="R78" s="8"/>
-      <c r="S78" s="8"/>
-      <c r="T78" s="8"/>
-      <c r="U78" s="8"/>
-      <c r="V78" s="8"/>
-      <c r="W78" s="8"/>
-      <c r="X78" s="8"/>
-      <c r="Y78" s="8"/>
+      <c r="Q78" s="23"/>
+      <c r="R78" s="23"/>
+      <c r="S78" s="23"/>
+      <c r="T78" s="23"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="23"/>
+      <c r="W78" s="23"/>
+      <c r="X78" s="23"/>
+      <c r="Y78" s="12"/>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C79" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D79" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="E79" s="8" t="s">
+      <c r="E79" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="F79" s="8" t="s">
+      <c r="F79" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="G79" s="8" t="s">
+      <c r="G79" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="H79" s="8" t="s">
+      <c r="H79" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="I79" s="8" t="s">
+      <c r="I79" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="J79" s="8" t="s">
+      <c r="J79" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="K79" s="8" t="s">
+      <c r="K79" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="L79" s="8" t="s">
+      <c r="L79" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="M79" s="8" t="s">
+      <c r="M79" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="N79" s="8" t="s">
+      <c r="N79" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="O79" s="8" t="s">
+      <c r="O79" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="P79" s="8" t="s">
+      <c r="P79" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="Q79" s="8"/>
-      <c r="R79" s="8"/>
-      <c r="S79" s="8"/>
-      <c r="T79" s="8"/>
-      <c r="U79" s="8"/>
-      <c r="V79" s="8"/>
-      <c r="W79" s="8"/>
-      <c r="X79" s="8"/>
-      <c r="Y79" s="8"/>
+      <c r="Q79" s="23"/>
+      <c r="R79" s="23"/>
+      <c r="S79" s="23"/>
+      <c r="T79" s="23"/>
+      <c r="U79" s="23"/>
+      <c r="V79" s="23"/>
+      <c r="W79" s="23"/>
+      <c r="X79" s="23"/>
+      <c r="Y79" s="12"/>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E80" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="F80" s="8" t="s">
+      <c r="F80" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="G80" s="8" t="s">
+      <c r="G80" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="H80" s="8" t="s">
+      <c r="H80" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="I80" s="8" t="s">
+      <c r="I80" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="J80" s="8" t="s">
+      <c r="J80" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="K80" s="8" t="s">
+      <c r="K80" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="L80" s="8" t="s">
+      <c r="L80" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="M80" s="8" t="s">
+      <c r="M80" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="N80" s="8" t="s">
+      <c r="N80" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="O80" s="8" t="s">
+      <c r="O80" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="P80" s="8" t="s">
+      <c r="P80" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="Q80" s="8"/>
-      <c r="R80" s="8"/>
-      <c r="S80" s="8"/>
-      <c r="T80" s="8"/>
-      <c r="U80" s="8"/>
-      <c r="V80" s="8"/>
-      <c r="W80" s="8"/>
-      <c r="X80" s="8"/>
-      <c r="Y80" s="8"/>
+      <c r="Q80" s="23"/>
+      <c r="R80" s="23"/>
+      <c r="S80" s="23"/>
+      <c r="T80" s="23"/>
+      <c r="U80" s="23"/>
+      <c r="V80" s="23"/>
+      <c r="W80" s="23"/>
+      <c r="X80" s="23"/>
+      <c r="Y80" s="12"/>
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="E81" s="8" t="s">
+      <c r="E81" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="F81" s="8" t="s">
+      <c r="F81" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="G81" s="8" t="s">
+      <c r="G81" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="H81" s="8" t="s">
+      <c r="H81" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="I81" s="8" t="s">
+      <c r="I81" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="J81" s="8" t="s">
+      <c r="J81" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="K81" s="8" t="s">
+      <c r="K81" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="L81" s="8" t="s">
+      <c r="L81" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="M81" s="8" t="s">
+      <c r="M81" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="N81" s="8" t="s">
+      <c r="N81" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="O81" s="8" t="s">
+      <c r="O81" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="P81" s="8" t="s">
+      <c r="P81" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="Q81" s="8" t="s">
+      <c r="Q81" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R81" s="8" t="s">
+      <c r="R81" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S81" s="8" t="s">
+      <c r="S81" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T81" s="8"/>
-      <c r="U81" s="8"/>
-      <c r="V81" s="8"/>
-      <c r="W81" s="8"/>
-      <c r="X81" s="8"/>
-      <c r="Y81" s="8"/>
+      <c r="T81" s="23"/>
+      <c r="U81" s="23"/>
+      <c r="V81" s="23"/>
+      <c r="W81" s="23"/>
+      <c r="X81" s="23"/>
+      <c r="Y81" s="12"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="E82" s="8" t="s">
+      <c r="E82" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="G82" s="8" t="s">
+      <c r="G82" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="H82" s="8" t="s">
+      <c r="H82" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="I82" s="8" t="s">
+      <c r="I82" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="J82" s="8" t="s">
+      <c r="J82" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="K82" s="8" t="s">
+      <c r="K82" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="L82" s="8" t="s">
+      <c r="L82" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="M82" s="8" t="s">
+      <c r="M82" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="N82" s="8" t="s">
+      <c r="N82" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="O82" s="8" t="s">
+      <c r="O82" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="P82" s="8" t="s">
+      <c r="P82" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="Q82" s="8" t="s">
+      <c r="Q82" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R82" s="8" t="s">
+      <c r="R82" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S82" s="8" t="s">
+      <c r="S82" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T82" s="8"/>
-      <c r="U82" s="8"/>
-      <c r="V82" s="8"/>
-      <c r="W82" s="8"/>
-      <c r="X82" s="8"/>
-      <c r="Y82" s="8"/>
+      <c r="T82" s="23"/>
+      <c r="U82" s="23"/>
+      <c r="V82" s="23"/>
+      <c r="W82" s="23"/>
+      <c r="X82" s="23"/>
+      <c r="Y82" s="12"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D83" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="E83" s="8" t="s">
+      <c r="E83" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="F83" s="8" t="s">
+      <c r="F83" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="G83" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="H83" s="8" t="s">
+      <c r="H83" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="I83" s="8" t="s">
+      <c r="I83" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="J83" s="8" t="s">
+      <c r="J83" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="K83" s="8" t="s">
+      <c r="K83" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="L83" s="8" t="s">
+      <c r="L83" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="M83" s="8" t="s">
+      <c r="M83" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="N83" s="8" t="s">
+      <c r="N83" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="O83" s="8" t="s">
+      <c r="O83" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="P83" s="8" t="s">
+      <c r="P83" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="Q83" s="8" t="s">
+      <c r="Q83" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R83" s="8" t="s">
+      <c r="R83" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S83" s="8" t="s">
+      <c r="S83" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T83" s="8"/>
-      <c r="U83" s="8"/>
-      <c r="V83" s="8"/>
-      <c r="W83" s="8"/>
-      <c r="X83" s="8"/>
-      <c r="Y83" s="8"/>
+      <c r="T83" s="23"/>
+      <c r="U83" s="23"/>
+      <c r="V83" s="23"/>
+      <c r="W83" s="23"/>
+      <c r="X83" s="23"/>
+      <c r="Y83" s="12"/>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D84" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F84" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="G84" s="8" t="s">
+      <c r="G84" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="H84" s="8" t="s">
+      <c r="H84" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="I84" s="8" t="s">
+      <c r="I84" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="J84" s="8" t="s">
+      <c r="J84" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="K84" s="8" t="s">
+      <c r="K84" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="L84" s="8" t="s">
+      <c r="L84" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="M84" s="8" t="s">
+      <c r="M84" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="N84" s="8" t="s">
+      <c r="N84" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="O84" s="8" t="s">
+      <c r="O84" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="P84" s="8" t="s">
+      <c r="P84" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="Q84" s="8" t="s">
+      <c r="Q84" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R84" s="8" t="s">
+      <c r="R84" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S84" s="8" t="s">
+      <c r="S84" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T84" s="8"/>
-      <c r="U84" s="8"/>
-      <c r="V84" s="8"/>
-      <c r="W84" s="8"/>
-      <c r="X84" s="8"/>
-      <c r="Y84" s="8"/>
+      <c r="T84" s="23"/>
+      <c r="U84" s="23"/>
+      <c r="V84" s="23"/>
+      <c r="W84" s="23"/>
+      <c r="X84" s="23"/>
+      <c r="Y84" s="12"/>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D85" s="23" t="s">
         <v>415</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E85" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="F85" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="G85" s="8" t="s">
+      <c r="G85" s="23" t="s">
         <v>418</v>
       </c>
-      <c r="H85" s="8" t="s">
+      <c r="H85" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="I85" s="8" t="s">
+      <c r="I85" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="J85" s="8" t="s">
+      <c r="J85" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="K85" s="8" t="s">
+      <c r="K85" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="L85" s="8" t="s">
+      <c r="L85" s="23" t="s">
         <v>423</v>
       </c>
-      <c r="M85" s="8" t="s">
+      <c r="M85" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="N85" s="8" t="s">
+      <c r="N85" s="23" t="s">
         <v>425</v>
       </c>
-      <c r="O85" s="8" t="s">
+      <c r="O85" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="P85" s="8" t="s">
+      <c r="P85" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="Q85" s="8" t="s">
+      <c r="Q85" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R85" s="8" t="s">
+      <c r="R85" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S85" s="8" t="s">
+      <c r="S85" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T85" s="8"/>
-      <c r="U85" s="8"/>
-      <c r="V85" s="8"/>
-      <c r="W85" s="8"/>
-      <c r="X85" s="8"/>
-      <c r="Y85" s="8"/>
+      <c r="T85" s="23"/>
+      <c r="U85" s="23"/>
+      <c r="V85" s="23"/>
+      <c r="W85" s="23"/>
+      <c r="X85" s="23"/>
+      <c r="Y85" s="12"/>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D86" s="23" t="s">
         <v>415</v>
       </c>
-      <c r="E86" s="8" t="s">
+      <c r="E86" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="F86" s="8" t="s">
+      <c r="F86" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="G86" s="8" t="s">
+      <c r="G86" s="23" t="s">
         <v>418</v>
       </c>
-      <c r="H86" s="8" t="s">
+      <c r="H86" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="I86" s="8" t="s">
+      <c r="I86" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="J86" s="8" t="s">
+      <c r="J86" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="K86" s="8" t="s">
+      <c r="K86" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="L86" s="8" t="s">
+      <c r="L86" s="23" t="s">
         <v>423</v>
       </c>
-      <c r="M86" s="8" t="s">
+      <c r="M86" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="N86" s="8" t="s">
+      <c r="N86" s="23" t="s">
         <v>425</v>
       </c>
-      <c r="O86" s="8" t="s">
+      <c r="O86" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="P86" s="8" t="s">
+      <c r="P86" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="Q86" s="8" t="s">
+      <c r="Q86" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R86" s="8" t="s">
+      <c r="R86" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S86" s="8" t="s">
+      <c r="S86" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T86" s="8"/>
-      <c r="U86" s="8"/>
-      <c r="V86" s="8"/>
-      <c r="W86" s="8"/>
-      <c r="X86" s="8"/>
-      <c r="Y86" s="8"/>
+      <c r="T86" s="23"/>
+      <c r="U86" s="23"/>
+      <c r="V86" s="23"/>
+      <c r="W86" s="23"/>
+      <c r="X86" s="23"/>
+      <c r="Y86" s="12"/>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="23" t="s">
         <v>415</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F87" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="G87" s="8" t="s">
+      <c r="G87" s="23" t="s">
         <v>418</v>
       </c>
-      <c r="H87" s="8" t="s">
+      <c r="H87" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="I87" s="8" t="s">
+      <c r="I87" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="J87" s="8" t="s">
+      <c r="J87" s="23" t="s">
         <v>421</v>
       </c>
-      <c r="K87" s="8" t="s">
+      <c r="K87" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="L87" s="8" t="s">
+      <c r="L87" s="23" t="s">
         <v>423</v>
       </c>
-      <c r="M87" s="8" t="s">
+      <c r="M87" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="N87" s="8" t="s">
+      <c r="N87" s="23" t="s">
         <v>425</v>
       </c>
-      <c r="O87" s="8" t="s">
+      <c r="O87" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="P87" s="8" t="s">
+      <c r="P87" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="Q87" s="8" t="s">
+      <c r="Q87" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="R87" s="8" t="s">
+      <c r="R87" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="S87" s="8" t="s">
+      <c r="S87" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="T87" s="8"/>
-      <c r="U87" s="8"/>
-      <c r="V87" s="8"/>
-      <c r="W87" s="8"/>
-      <c r="X87" s="8"/>
-      <c r="Y87" s="8"/>
+      <c r="T87" s="23"/>
+      <c r="U87" s="23"/>
+      <c r="V87" s="23"/>
+      <c r="W87" s="23"/>
+      <c r="X87" s="23"/>
+      <c r="Y87" s="12"/>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D88" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E88" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="F88" s="8" t="s">
+      <c r="F88" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="G88" s="8" t="s">
+      <c r="G88" s="14" t="s">
         <v>418</v>
       </c>
-      <c r="H88" s="8" t="s">
+      <c r="H88" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="I88" s="8" t="s">
+      <c r="I88" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="J88" s="8" t="s">
+      <c r="J88" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="K88" s="8" t="s">
+      <c r="K88" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="L88" s="8" t="s">
+      <c r="L88" s="14" t="s">
         <v>423</v>
       </c>
-      <c r="M88" s="8" t="s">
+      <c r="M88" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="N88" s="8" t="s">
+      <c r="N88" s="14" t="s">
         <v>425</v>
       </c>
-      <c r="O88" s="8" t="s">
+      <c r="O88" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="P88" s="8" t="s">
+      <c r="P88" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="Q88" s="8" t="s">
+      <c r="Q88" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="R88" s="8" t="s">
+      <c r="R88" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="S88" s="8" t="s">
+      <c r="S88" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="T88" s="8"/>
-      <c r="U88" s="8"/>
-      <c r="V88" s="8"/>
-      <c r="W88" s="8"/>
-      <c r="X88" s="8"/>
-      <c r="Y88" s="8"/>
+      <c r="T88" s="14"/>
+      <c r="U88" s="14"/>
+      <c r="V88" s="14"/>
+      <c r="W88" s="14"/>
+      <c r="X88" s="14"/>
+      <c r="Y88" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6257,7 +6260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:JF80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>

</xml_diff>